<commit_message>
melon crawling 중복 제거 작업
</commit_message>
<xml_diff>
--- a/celeb/melon_singer.xlsx
+++ b/celeb/melon_singer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,16 +561,16 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>NewJeans</t>
+          <t>윤하 (YOUNHA)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3114174</t>
+          <t>203912</t>
         </is>
       </c>
     </row>
@@ -578,22 +578,18 @@
       <c r="A8" t="n">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-민지(MINJI)
-</t>
+          <t>LE SSERAFIM (르세라핌)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3116664</t>
+          <t>3092950</t>
         </is>
       </c>
     </row>
@@ -602,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
         <v>7</v>
@@ -610,13 +606,13 @@
       <c r="D9" t="inlineStr">
         <is>
           <t xml:space="preserve">
-하니(HANNI)
+김채원
 </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3116665</t>
+          <t>2399729</t>
         </is>
       </c>
     </row>
@@ -625,7 +621,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n">
         <v>7</v>
@@ -633,13 +629,13 @@
       <c r="D10" t="inlineStr">
         <is>
           <t xml:space="preserve">
-다니엘(DANIELLE)
+미야와키 사쿠라
 </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3116666</t>
+          <t>2399720</t>
         </is>
       </c>
     </row>
@@ -648,7 +644,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" t="n">
         <v>7</v>
@@ -656,13 +652,13 @@
       <c r="D11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-해린(HAERIN)
+허윤진
 </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3116671</t>
+          <t>3093330</t>
         </is>
       </c>
     </row>
@@ -671,7 +667,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" t="n">
         <v>7</v>
@@ -679,13 +675,13 @@
       <c r="D12" t="inlineStr">
         <is>
           <t xml:space="preserve">
-혜인(HYEIN)
+카즈하
 </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3116674</t>
+          <t>3093335</t>
         </is>
       </c>
     </row>
@@ -693,18 +689,22 @@
       <c r="A13" t="n">
         <v>13</v>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>8</v>
+      </c>
       <c r="C13" t="n">
         <v>7</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>NewJeans</t>
+          <t xml:space="preserve">
+홍은채
+</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3114174</t>
+          <t>3093339</t>
         </is>
       </c>
     </row>
@@ -712,22 +712,18 @@
       <c r="A14" t="n">
         <v>14</v>
       </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-민지(MINJI)
-</t>
+          <t>이영지</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3116664</t>
+          <t>2636153</t>
         </is>
       </c>
     </row>
@@ -735,22 +731,18 @@
       <c r="A15" t="n">
         <v>15</v>
       </c>
-      <c r="B15" t="n">
-        <v>13</v>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
         <v>7</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-하니(HANNI)
-</t>
+          <t>IVE (아이브)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3116665</t>
+          <t>3055146</t>
         </is>
       </c>
     </row>
@@ -759,7 +751,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" t="n">
         <v>7</v>
@@ -767,13 +759,13 @@
       <c r="D16" t="inlineStr">
         <is>
           <t xml:space="preserve">
-다니엘(DANIELLE)
+안유진 (IVE)
 </t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3116666</t>
+          <t>2399726</t>
         </is>
       </c>
     </row>
@@ -782,7 +774,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17" t="n">
         <v>7</v>
@@ -790,13 +782,13 @@
       <c r="D17" t="inlineStr">
         <is>
           <t xml:space="preserve">
-해린(HAERIN)
+가을 (IVE)
 </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3116671</t>
+          <t>3055166</t>
         </is>
       </c>
     </row>
@@ -805,7 +797,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C18" t="n">
         <v>7</v>
@@ -813,13 +805,13 @@
       <c r="D18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-혜인(HYEIN)
+레이 (IVE)
 </t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3116674</t>
+          <t>3055169</t>
         </is>
       </c>
     </row>
@@ -827,18 +819,22 @@
       <c r="A19" t="n">
         <v>19</v>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>15</v>
+      </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>윤하 (YOUNHA)</t>
+          <t xml:space="preserve">
+장원영 (IVE)
+</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>203912</t>
+          <t>2399717</t>
         </is>
       </c>
     </row>
@@ -846,18 +842,22 @@
       <c r="A20" t="n">
         <v>20</v>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>15</v>
+      </c>
       <c r="C20" t="n">
         <v>7</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>LE SSERAFIM (르세라핌)</t>
+          <t xml:space="preserve">
+리즈 (IVE)
+</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3092950</t>
+          <t>3055170</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C21" t="n">
         <v>7</v>
@@ -874,13 +874,13 @@
       <c r="D21" t="inlineStr">
         <is>
           <t xml:space="preserve">
-김채원
+이서 (IVE)
 </t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2399729</t>
+          <t>3055172</t>
         </is>
       </c>
     </row>
@@ -888,22 +888,18 @@
       <c r="A22" t="n">
         <v>22</v>
       </c>
-      <c r="B22" t="n">
-        <v>20</v>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-미야와키 사쿠라
-</t>
+          <t>NCT DREAM</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2399720</t>
+          <t>1066419</t>
         </is>
       </c>
     </row>
@@ -912,21 +908,21 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
           <t xml:space="preserve">
-허윤진
+천러 (CHENLE)
 </t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3093330</t>
+          <t>1066422</t>
         </is>
       </c>
     </row>
@@ -935,21 +931,21 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
           <t xml:space="preserve">
-카즈하
+런쥔 (RENJUN)
 </t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3093335</t>
+          <t>1066423</t>
         </is>
       </c>
     </row>
@@ -958,21 +954,21 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C25" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t xml:space="preserve">
-홍은채
+재민 (JAEMIN)
 </t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3093339</t>
+          <t>1066424</t>
         </is>
       </c>
     </row>
@@ -980,18 +976,2798 @@
       <c r="A26" t="n">
         <v>26</v>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="n">
+        <v>22</v>
+      </c>
       <c r="C26" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>이영지</t>
+          <t xml:space="preserve">
+지성 (JISUNG)
+</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2636153</t>
+          <t>1066427</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>27</v>
+      </c>
+      <c r="B27" t="n">
+        <v>22</v>
+      </c>
+      <c r="C27" t="n">
+        <v>8</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+제노 (JENO)
+</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1066430</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>28</v>
+      </c>
+      <c r="B28" t="n">
+        <v>22</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+해찬 (HAECHAN)
+</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>991416</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" t="n">
+        <v>22</v>
+      </c>
+      <c r="C29" t="n">
+        <v>8</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+마크 (MARK)
+</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>965986</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>7</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>(여자)아이들</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2137482</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>31</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>7</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+전소연
+</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1050107</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>7</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+미연 ((여자)아이들)
+</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2138414</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>33</v>
+      </c>
+      <c r="B33" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" t="n">
+        <v>7</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+우기 ((여자)아이들)
+</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2138416</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>34</v>
+      </c>
+      <c r="B34" t="n">
+        <v>30</v>
+      </c>
+      <c r="C34" t="n">
+        <v>7</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+슈화 ((여자)아이들)
+</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2138418</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>35</v>
+      </c>
+      <c r="B35" t="n">
+        <v>30</v>
+      </c>
+      <c r="C35" t="n">
+        <v>7</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+민니 ((여자)아이들)
+</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2138419</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>36</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="n">
+        <v>10</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>지코 (ZICO)</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>602056</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>37</v>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="n">
+        <v>10</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>테이</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>51893</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>38</v>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>10</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>저스디스 (JUSTHIS)</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>786499</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>39</v>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>R.Tee</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>633071</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>40</v>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>던말릭 (DON MALIK)</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>789943</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>41</v>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>10</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>허성현 (Huh)</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2190397</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>42</v>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="n">
+        <v>10</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>KHAN</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2741140</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>43</v>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>10</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>맥대디 (Mckdaddy)</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>774027</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>44</v>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="n">
+        <v>10</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>로스 (Los)</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>1628539</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>45</v>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="n">
+        <v>10</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>성시경</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>3305</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>46</v>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="n">
+        <v>10</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>태양</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>247621</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>47</v>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="n">
+        <v>10</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>송하예</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>722098</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>48</v>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="n">
+        <v>10</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>#안녕</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>1024489</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>49</v>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="n">
+        <v>10</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>임영웅</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>994944</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>50</v>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="n">
+        <v>7</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>BLACKPINK</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>995169</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>51</v>
+      </c>
+      <c r="B51" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" t="n">
+        <v>7</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+지수 (JISOO)
+</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>995174</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>52</v>
+      </c>
+      <c r="B52" t="n">
+        <v>50</v>
+      </c>
+      <c r="C52" t="n">
+        <v>7</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+제니 (JENNIE)
+</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>995173</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>53</v>
+      </c>
+      <c r="B53" t="n">
+        <v>50</v>
+      </c>
+      <c r="C53" t="n">
+        <v>7</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+로제 (ROSÉ)
+</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>995171</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>54</v>
+      </c>
+      <c r="B54" t="n">
+        <v>50</v>
+      </c>
+      <c r="C54" t="n">
+        <v>7</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+리사 (LISA)
+</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>995172</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>55</v>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="n">
+        <v>8</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>멜로망스</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>839732</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>56</v>
+      </c>
+      <c r="B56" t="n">
+        <v>55</v>
+      </c>
+      <c r="C56" t="n">
+        <v>8</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+정동환 (멜로망스)
+</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>839735</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>57</v>
+      </c>
+      <c r="B57" t="n">
+        <v>55</v>
+      </c>
+      <c r="C57" t="n">
+        <v>8</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+김민석 (멜로망스)
+</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>839736</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>58</v>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>10</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>주호</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>683631</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>59</v>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>10</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Crush</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>674710</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>60</v>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>10</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>우디 (Woody)</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>673033</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>61</v>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="n">
+        <v>7</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>WSG워너비 (가야G)</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>3110856</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>62</v>
+      </c>
+      <c r="B62" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" t="n">
+        <v>7</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+이보람 (씨야)
+</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>46751</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>63</v>
+      </c>
+      <c r="B63" t="n">
+        <v>61</v>
+      </c>
+      <c r="C63" t="n">
+        <v>7</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+소연 (LABOUM)
+</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>784317</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>64</v>
+      </c>
+      <c r="B64" t="n">
+        <v>61</v>
+      </c>
+      <c r="C64" t="n">
+        <v>7</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+HYNN (박혜원)
+</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>1229685</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>65</v>
+      </c>
+      <c r="B65" t="n">
+        <v>61</v>
+      </c>
+      <c r="C65" t="n">
+        <v>7</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+정지소
+</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>3101554</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>66</v>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>10</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>정국</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>725987</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>67</v>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>8</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>방탄소년단</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>672375</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>68</v>
+      </c>
+      <c r="B68" t="n">
+        <v>67</v>
+      </c>
+      <c r="C68" t="n">
+        <v>8</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+RM
+</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>725991</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>69</v>
+      </c>
+      <c r="B69" t="n">
+        <v>67</v>
+      </c>
+      <c r="C69" t="n">
+        <v>8</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+SUGA
+</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>725988</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>70</v>
+      </c>
+      <c r="B70" t="n">
+        <v>67</v>
+      </c>
+      <c r="C70" t="n">
+        <v>8</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+진
+</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>725986</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>71</v>
+      </c>
+      <c r="B71" t="n">
+        <v>67</v>
+      </c>
+      <c r="C71" t="n">
+        <v>8</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+j-hope
+</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>725984</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>72</v>
+      </c>
+      <c r="B72" t="n">
+        <v>67</v>
+      </c>
+      <c r="C72" t="n">
+        <v>8</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+지민
+</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>725985</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>73</v>
+      </c>
+      <c r="B73" t="n">
+        <v>67</v>
+      </c>
+      <c r="C73" t="n">
+        <v>8</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+V
+</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>725989</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>74</v>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="n">
+        <v>10</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>BE'O (비오)</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2758756</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>75</v>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="n">
+        <v>10</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>10CM</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>468244</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>76</v>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="n">
+        <v>10</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>BIG Naughty (서동현)</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2744750</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>77</v>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="n">
+        <v>10</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Charlie Puth</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>838654</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>78</v>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="n">
+        <v>10</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>최유리</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2645970</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>79</v>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="n">
+        <v>10</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>경서</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>994005</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>80</v>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="n">
+        <v>7</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>카라</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>222128</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>81</v>
+      </c>
+      <c r="B81" t="n">
+        <v>80</v>
+      </c>
+      <c r="C81" t="n">
+        <v>7</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+박규리 (카라)
+</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>204065</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>82</v>
+      </c>
+      <c r="B82" t="n">
+        <v>80</v>
+      </c>
+      <c r="C82" t="n">
+        <v>7</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+한승연
+</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>407540</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>83</v>
+      </c>
+      <c r="B83" t="n">
+        <v>80</v>
+      </c>
+      <c r="C83" t="n">
+        <v>7</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+구하라 (카라)
+</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>556401</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>84</v>
+      </c>
+      <c r="B84" t="n">
+        <v>80</v>
+      </c>
+      <c r="C84" t="n">
+        <v>7</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+허영지 (카라)
+</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>778238</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>85</v>
+      </c>
+      <c r="B85" t="n">
+        <v>80</v>
+      </c>
+      <c r="C85" t="n">
+        <v>7</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+니콜
+</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>408880</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>86</v>
+      </c>
+      <c r="B86" t="n">
+        <v>80</v>
+      </c>
+      <c r="C86" t="n">
+        <v>7</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+강지영
+</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>512342</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>87</v>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="n">
+        <v>7</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>경서예지</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2863470</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>88</v>
+      </c>
+      <c r="B88" t="n">
+        <v>87</v>
+      </c>
+      <c r="C88" t="n">
+        <v>7</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+경서 (경서예지)
+</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2917776</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>89</v>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="n">
+        <v>10</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>전건호</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2739011</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>90</v>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="n">
+        <v>10</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>폴킴</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>752425</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>91</v>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="n">
+        <v>7</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>WSG워너비(4FIRE)</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>3110857</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>92</v>
+      </c>
+      <c r="B92" t="n">
+        <v>91</v>
+      </c>
+      <c r="C92" t="n">
+        <v>7</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+나비 (Navi)
+</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>242868</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>93</v>
+      </c>
+      <c r="B93" t="n">
+        <v>91</v>
+      </c>
+      <c r="C93" t="n">
+        <v>7</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+SOLE (쏠)
+</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2006587</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>94</v>
+      </c>
+      <c r="B94" t="n">
+        <v>91</v>
+      </c>
+      <c r="C94" t="n">
+        <v>7</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+엄지윤
+</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>3101553</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>95</v>
+      </c>
+      <c r="B95" t="n">
+        <v>91</v>
+      </c>
+      <c r="C95" t="n">
+        <v>7</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+권진아
+</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>760046</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>96</v>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="n">
+        <v>10</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>백아</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2113114</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>97</v>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="n">
+        <v>10</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>임한별</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>471741</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>98</v>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>강민경 (다비치)</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>261742</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>99</v>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="n">
+        <v>10</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>잔나비 최정훈</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>772258</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>100</v>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="n">
+        <v>10</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>The Kid LAROI</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2743730</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>101</v>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="n">
+        <v>10</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Justin Bieber</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>420621</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>102</v>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="n">
+        <v>10</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>김승민</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>827322</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>103</v>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="n">
+        <v>10</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Sia</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>54103</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>104</v>
+      </c>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="n">
+        <v>10</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>한동근</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>711476</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>105</v>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="n">
+        <v>10</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>싸이 (PSY)</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>3865</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>106</v>
+      </c>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="n">
+        <v>10</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>이무진</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2138620</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>107</v>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="n">
+        <v>8</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>BIGBANG (빅뱅)</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>198094</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>108</v>
+      </c>
+      <c r="B108" t="n">
+        <v>107</v>
+      </c>
+      <c r="C108" t="n">
+        <v>8</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+G-DRAGON
+</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>6984</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>109</v>
+      </c>
+      <c r="B109" t="n">
+        <v>107</v>
+      </c>
+      <c r="C109" t="n">
+        <v>8</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+대성
+</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>251080</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>110</v>
+      </c>
+      <c r="B110" t="n">
+        <v>107</v>
+      </c>
+      <c r="C110" t="n">
+        <v>8</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+T.O.P
+</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>152192</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>111</v>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="n">
+        <v>8</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>잔나비</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>772253</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>112</v>
+      </c>
+      <c r="B112" t="n">
+        <v>111</v>
+      </c>
+      <c r="C112" t="n">
+        <v>8</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+김도형
+</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>772255</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>113</v>
+      </c>
+      <c r="B113" t="n">
+        <v>111</v>
+      </c>
+      <c r="C113" t="n">
+        <v>8</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+장경준
+</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>861835</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>114</v>
+      </c>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="n">
+        <v>8</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>그루비룸 (GroovyRoom)</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>858851</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>115</v>
+      </c>
+      <c r="B115" t="n">
+        <v>114</v>
+      </c>
+      <c r="C115" t="n">
+        <v>8</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Lil Moshpit
+</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>776579</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>116</v>
+      </c>
+      <c r="B116" t="n">
+        <v>114</v>
+      </c>
+      <c r="C116" t="n">
+        <v>8</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+박규정
+</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>946280</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>117</v>
+      </c>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="n">
+        <v>10</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>릴보이 (lIlBOI)</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>623251</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>118</v>
+      </c>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="n">
+        <v>10</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Blase (블라세)</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2113072</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>119</v>
+      </c>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="n">
+        <v>10</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>노윤하</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>2928842</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>120</v>
+      </c>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="n">
+        <v>10</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Polodared</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2971357</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>121</v>
+      </c>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="n">
+        <v>10</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Chillin Homie</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2296594</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>122</v>
+      </c>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="n">
+        <v>10</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Fleeky Bang</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>3089953</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>123</v>
+      </c>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="n">
+        <v>10</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>볼빨간사춘기</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>792022</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>124</v>
+      </c>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="n">
+        <v>7</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>소녀시대 (GIRLS' GENERATION)</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>228069</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>125</v>
+      </c>
+      <c r="B125" t="n">
+        <v>124</v>
+      </c>
+      <c r="C125" t="n">
+        <v>7</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+태연 (TAEYEON)
+</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>236797</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>126</v>
+      </c>
+      <c r="B126" t="n">
+        <v>124</v>
+      </c>
+      <c r="C126" t="n">
+        <v>7</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+써니 (SUNNY)
+</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>257449</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>127</v>
+      </c>
+      <c r="B127" t="n">
+        <v>124</v>
+      </c>
+      <c r="C127" t="n">
+        <v>7</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+유리 (YURI)
+</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>428786</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>128</v>
+      </c>
+      <c r="B128" t="n">
+        <v>124</v>
+      </c>
+      <c r="C128" t="n">
+        <v>7</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+수영 (SOOYOUNG)
+</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>428787</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>129</v>
+      </c>
+      <c r="B129" t="n">
+        <v>124</v>
+      </c>
+      <c r="C129" t="n">
+        <v>7</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Tiffany Young
+</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>406421</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>130</v>
+      </c>
+      <c r="B130" t="n">
+        <v>124</v>
+      </c>
+      <c r="C130" t="n">
+        <v>7</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+서현 (SEOHYUN)
+</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>401220</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>131</v>
+      </c>
+      <c r="B131" t="n">
+        <v>124</v>
+      </c>
+      <c r="C131" t="n">
+        <v>7</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+윤아 (YOONA)
+</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>429140</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>132</v>
+      </c>
+      <c r="B132" t="n">
+        <v>124</v>
+      </c>
+      <c r="C132" t="n">
+        <v>7</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+효연 (HYOYEON)
+</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>435380</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>133</v>
+      </c>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="n">
+        <v>7</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>aespa</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>2899555</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>134</v>
+      </c>
+      <c r="B134" t="n">
+        <v>133</v>
+      </c>
+      <c r="C134" t="n">
+        <v>7</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+카리나 (KARINA)
+</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>2899557</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>135</v>
+      </c>
+      <c r="B135" t="n">
+        <v>133</v>
+      </c>
+      <c r="C135" t="n">
+        <v>7</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+지젤 (GISELLE)
+</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>2899559</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>136</v>
+      </c>
+      <c r="B136" t="n">
+        <v>133</v>
+      </c>
+      <c r="C136" t="n">
+        <v>7</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+윈터 (WINTER)
+</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>2899560</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>137</v>
+      </c>
+      <c r="B137" t="n">
+        <v>133</v>
+      </c>
+      <c r="C137" t="n">
+        <v>7</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+닝닝 (NINGNING)
+</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>2899561</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>138</v>
+      </c>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="n">
+        <v>8</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>엠씨더맥스 (M.C the MAX)</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>161636</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>139</v>
+      </c>
+      <c r="B139" t="n">
+        <v>138</v>
+      </c>
+      <c r="C139" t="n">
+        <v>8</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+이수 (엠씨더맥스)
+</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>214784</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>140</v>
+      </c>
+      <c r="B140" t="n">
+        <v>138</v>
+      </c>
+      <c r="C140" t="n">
+        <v>8</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+전민혁
+</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>1935</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>141</v>
+      </c>
+      <c r="B141" t="n">
+        <v>138</v>
+      </c>
+      <c r="C141" t="n">
+        <v>8</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+J. Yoon
+</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>1934</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>142</v>
+      </c>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="n">
+        <v>10</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>신예영</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>2740042</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>143</v>
+      </c>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="n">
+        <v>10</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>아이유</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>261143</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>144</v>
+      </c>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="n">
+        <v>10</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Sam Smith</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>718042</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>145</v>
+      </c>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="n">
+        <v>10</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Kim Petras</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>2559079</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>146</v>
+      </c>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="n">
+        <v>7</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>ITZY (있지)</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>2622030</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>147</v>
+      </c>
+      <c r="B147" t="n">
+        <v>146</v>
+      </c>
+      <c r="C147" t="n">
+        <v>7</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+예지 (ITZY)
+</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>2622592</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>148</v>
+      </c>
+      <c r="B148" t="n">
+        <v>146</v>
+      </c>
+      <c r="C148" t="n">
+        <v>7</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+리아 (ITZY)
+</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>2622593</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>149</v>
+      </c>
+      <c r="B149" t="n">
+        <v>146</v>
+      </c>
+      <c r="C149" t="n">
+        <v>7</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+류진 (ITZY)
+</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>2622594</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>150</v>
+      </c>
+      <c r="B150" t="n">
+        <v>146</v>
+      </c>
+      <c r="C150" t="n">
+        <v>7</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+채령 (ITZY)
+</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>2622595</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>151</v>
+      </c>
+      <c r="B151" t="n">
+        <v>146</v>
+      </c>
+      <c r="C151" t="n">
+        <v>7</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+유나 (ITZY)
+</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>2622596</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>152</v>
+      </c>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="n">
+        <v>7</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Red Velvet (레드벨벳)</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>780066</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>153</v>
+      </c>
+      <c r="B153" t="n">
+        <v>152</v>
+      </c>
+      <c r="C153" t="n">
+        <v>7</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+웬디 (WENDY)
+</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>780915</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>154</v>
+      </c>
+      <c r="B154" t="n">
+        <v>152</v>
+      </c>
+      <c r="C154" t="n">
+        <v>7</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+아이린 (IRENE)
+</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>780918</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>155</v>
+      </c>
+      <c r="B155" t="n">
+        <v>152</v>
+      </c>
+      <c r="C155" t="n">
+        <v>7</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+슬기 (SEULGI)
+</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>780920</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>156</v>
+      </c>
+      <c r="B156" t="n">
+        <v>152</v>
+      </c>
+      <c r="C156" t="n">
+        <v>7</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+조이 (JOY)
+</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>780922</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>157</v>
+      </c>
+      <c r="B157" t="n">
+        <v>152</v>
+      </c>
+      <c r="C157" t="n">
+        <v>7</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+예리 (YERI)
+</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>856499</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>158</v>
+      </c>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="n">
+        <v>10</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>김연지</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>428803</t>
         </is>
       </c>
     </row>

</xml_diff>